<commit_message>
dimlex export; eval cont'ed, merging losses quantified; todo: change Moses2CoNLL to read OPUS ids.gz => faster and more reliable
</commit_message>
<xml_diff>
--- a/discourse-markers/parcor/opus/eval/eval-dimlex-disamb.xlsx
+++ b/discourse-markers/parcor/opus/eval/eval-dimlex-disamb.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="91">
   <si>
     <t>20:30:03.939902700</t>
   </si>
@@ -78,6 +78,12 @@
     <t>nsec/1000000 diff</t>
   </si>
   <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>hour</t>
+  </si>
+  <si>
     <t>minute</t>
   </si>
   <si>
@@ -226,17 +232,75 @@
   </si>
   <si>
     <t>dimlexing is slowed down by merging</t>
+  </si>
+  <si>
+    <t>12:56:30.685736500+01:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cf. </t>
+  </si>
+  <si>
+    <t>build.sh (2017-12-02)</t>
+  </si>
+  <si>
+    <t>given Europarl.en-de-it.conll with 380471 lines (incl. retok), 285573 tokens, 10143 sentences</t>
+  </si>
+  <si>
+    <t>user    0m8,381s</t>
+  </si>
+  <si>
+    <t>sys     0m13,209s</t>
+  </si>
+  <si>
+    <t>dimlex and disambiguate, no merge</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>no merge, Europarl.en-de-it.dimlexed_disamb.conll</t>
+  </si>
+  <si>
+    <t>14:22:29.309703900+01:00</t>
+  </si>
+  <si>
+    <t>14:27:32.387051300+01:00</t>
+  </si>
+  <si>
+    <t>error  (see txt for msg), I think we didn't loose time, but a data batch</t>
+  </si>
+  <si>
+    <t>that was much slower, but also, there may be less alignment errors, as this was done with merge -window=15000</t>
+  </si>
+  <si>
+    <t>14:32:06.478453100+01:00</t>
+  </si>
+  <si>
+    <t>14:33:23.318447300+01:00</t>
+  </si>
+  <si>
+    <t>14:35:11.622324900+01:00</t>
+  </si>
+  <si>
+    <t>15:15:30.402881900+01:00</t>
+  </si>
+  <si>
+    <t>15:55:36.431349000+01:00</t>
+  </si>
+  <si>
+    <t>16:28:24.933761100+01:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="168" formatCode="0.0000"/>
     <numFmt numFmtId="169" formatCode="0.00000"/>
     <numFmt numFmtId="171" formatCode="0.0000000"/>
+    <numFmt numFmtId="175" formatCode="#,##0.00000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -275,7 +339,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -292,6 +356,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,10 +416,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$U$6:$U$39</c:f>
+              <c:f>Sheet1!$U$6:$U$48</c:f>
               <c:numCache>
                 <c:formatCode>0.00000</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -456,16 +521,43 @@
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>14.196978859555557</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>16.440762731611112</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>17.873713833666667</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>17.95790198572222</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>18.034038486222222</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>18.055382929055558</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>18.085467339499999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>18.757350827555555</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>19.425692068416666</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>19.972498293999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$V$6:$V$39</c:f>
+              <c:f>Sheet1!$V$6:$V$48</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -567,6 +659,33 @@
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>309653.70969392027</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>361815.86620288127</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="General">
+                  <c:v>372496.78332604794</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="General">
+                  <c:v>373899.21410701168</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="General">
+                  <c:v>375076.67609118216</c:v>
+                </c:pt>
+                <c:pt idx="38" formatCode="General">
+                  <c:v>375504.06311325228</c:v>
+                </c:pt>
+                <c:pt idx="39" formatCode="General">
+                  <c:v>375961.51756401075</c:v>
+                </c:pt>
+                <c:pt idx="40" formatCode="General">
+                  <c:v>386620.95795239997</c:v>
+                </c:pt>
+                <c:pt idx="41" formatCode="General">
+                  <c:v>400768.22006863775</c:v>
+                </c:pt>
+                <c:pt idx="42" formatCode="General">
+                  <c:v>412276.52839910344</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -597,10 +716,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$U$6:$U$39</c:f>
+              <c:f>Sheet1!$U$6:$U$48</c:f>
               <c:numCache>
                 <c:formatCode>0.00000</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -702,16 +821,43 @@
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>14.196978859555557</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>16.440762731611112</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>17.873713833666667</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>17.95790198572222</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>18.034038486222222</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>18.055382929055558</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>18.085467339499999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>18.757350827555555</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>19.425692068416666</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>19.972498293999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$W$6:$W$39</c:f>
+              <c:f>Sheet1!$W$6:$W$48</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -813,6 +959,33 @@
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>305327.64591743954</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>357636.90330969269</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="General">
+                  <c:v>368224.70052736864</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="General">
+                  <c:v>369673.95330060011</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="General">
+                  <c:v>370870.48939807236</c:v>
+                </c:pt>
+                <c:pt idx="38" formatCode="General">
+                  <c:v>371194.89509001636</c:v>
+                </c:pt>
+                <c:pt idx="39" formatCode="General">
+                  <c:v>371704.45442807785</c:v>
+                </c:pt>
+                <c:pt idx="40" formatCode="General">
+                  <c:v>382312.88157846883</c:v>
+                </c:pt>
+                <c:pt idx="41" formatCode="General">
+                  <c:v>396667.18876159302</c:v>
+                </c:pt>
+                <c:pt idx="42" formatCode="General">
+                  <c:v>407897.60838334245</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -843,10 +1016,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$U$6:$U$39</c:f>
+              <c:f>Sheet1!$U$6:$U$48</c:f>
               <c:numCache>
                 <c:formatCode>0.00000</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -948,16 +1121,43 @@
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>14.196978859555557</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>16.440762731611112</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>17.873713833666667</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>17.95790198572222</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>18.034038486222222</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>18.055382929055558</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>18.085467339499999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>18.757350827555555</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>19.425692068416666</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>19.972498293999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$X$6:$X$39</c:f>
+              <c:f>Sheet1!$X$6:$X$48</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="34"/>
+                <c:ptCount val="43"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1059,6 +1259,33 @@
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>292176.5624164397</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>343494.15766278782</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="General">
+                  <c:v>355735.60846744245</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="General">
+                  <c:v>357713.1669225056</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="General">
+                  <c:v>357713.1669225056</c:v>
+                </c:pt>
+                <c:pt idx="38" formatCode="General">
+                  <c:v>357713.1669225056</c:v>
+                </c:pt>
+                <c:pt idx="39" formatCode="General">
+                  <c:v>359610.4658083684</c:v>
+                </c:pt>
+                <c:pt idx="40" formatCode="General">
+                  <c:v>372081.49631096807</c:v>
+                </c:pt>
+                <c:pt idx="41" formatCode="General">
+                  <c:v>387408.27427581087</c:v>
+                </c:pt>
+                <c:pt idx="42" formatCode="General">
+                  <c:v>398934.8549641</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1458,10 +1685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D1:AC206"/>
+  <dimension ref="D1:AH206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E6" workbookViewId="0">
-      <selection activeCell="X7" sqref="X7"/>
+    <sheetView tabSelected="1" topLeftCell="E41" workbookViewId="0">
+      <selection activeCell="X48" sqref="X48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1484,12 +1711,12 @@
     <col min="29" max="29" width="9.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:29" x14ac:dyDescent="0.35">
+    <row r="1" spans="4:34" x14ac:dyDescent="0.35">
       <c r="F1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>16</v>
@@ -1498,34 +1725,34 @@
         <v>17</v>
       </c>
       <c r="O1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="P1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="Q1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="R1" s="6" t="s">
         <v>19</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="U1" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="V1" s="6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="Y1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="Z1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="AA1" t="str">
         <f>V2</f>
@@ -1539,8 +1766,20 @@
         <f>X2</f>
         <v>Europarl.en-de-it.dimlexed_disamb.conll</v>
       </c>
-    </row>
-    <row r="2" spans="4:29" x14ac:dyDescent="0.35">
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="4:34" x14ac:dyDescent="0.35">
       <c r="F2" t="s">
         <v>6</v>
       </c>
@@ -1568,16 +1807,25 @@
         <v>Europarl.en-de-it.dimlexed_disamb.conll</v>
       </c>
       <c r="Y2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="4:29" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF2">
+        <v>285573</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="4:34" x14ac:dyDescent="0.35">
       <c r="M3" s="2"/>
       <c r="R3" s="6"/>
       <c r="S3" s="6"/>
       <c r="T3" s="6"/>
       <c r="U3" s="6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="V3">
         <v>230920</v>
@@ -1589,28 +1837,35 @@
         <v>207317</v>
       </c>
       <c r="Z3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="AA3" s="8">
         <f>(MAX(V6:V304)-V6)/(MAX($U6:$U304)-$U6)</f>
-        <v>21811.239754400405</v>
+        <v>20642.211221164893</v>
       </c>
       <c r="AB3" s="8">
         <f>(MAX(W6:W304)-W9)/(MAX($U6:$U304)-$U9)</f>
-        <v>21833.387122402652</v>
+        <v>20632.794628474978</v>
       </c>
       <c r="AC3" s="8">
         <f>(MAX(X6:X304)-X7)/(MAX($U6:$U304)-$U7)</f>
-        <v>20966.359667733228</v>
-      </c>
-    </row>
-    <row r="4" spans="4:29" x14ac:dyDescent="0.35">
+        <v>20235.550537799769</v>
+      </c>
+      <c r="AE3" s="8">
+        <f>AF2/AH6</f>
+        <v>15098.369192290849</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="4:34" x14ac:dyDescent="0.35">
       <c r="M4" s="2"/>
       <c r="R4" s="6"/>
       <c r="S4" s="6"/>
       <c r="T4" s="6"/>
       <c r="U4" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="V4">
         <v>430084</v>
@@ -1622,29 +1877,39 @@
         <v>222145</v>
       </c>
       <c r="Z4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AA4" s="11">
         <f>AA3/60</f>
-        <v>363.52066257334008</v>
+        <v>344.03685368608154</v>
       </c>
       <c r="AB4" s="11">
-        <f t="shared" ref="AB4:AC4" si="0">AB3/60</f>
-        <v>363.88978537337755</v>
+        <f t="shared" ref="AB4:AE4" si="0">AB3/60</f>
+        <v>343.87991047458297</v>
       </c>
       <c r="AC4" s="11">
         <f t="shared" si="0"/>
-        <v>349.43932779555382</v>
-      </c>
-    </row>
-    <row r="5" spans="4:29" x14ac:dyDescent="0.35">
+        <v>337.25917562999615</v>
+      </c>
+      <c r="AE4" s="11">
+        <f t="shared" si="0"/>
+        <v>251.63948653818082</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="4:34" x14ac:dyDescent="0.35">
       <c r="M5" s="2"/>
       <c r="R5" s="6"/>
       <c r="S5" s="6"/>
       <c r="T5" s="6"/>
       <c r="U5" s="6"/>
       <c r="Z5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="AA5" s="4">
         <f>-(((MAX(V6:V304)-MAX($U6:$U304)*AA3)))/AA3</f>
@@ -1652,14 +1917,20 @@
       </c>
       <c r="AB5" s="3">
         <f>-(((MAX(W6:W304)-MAX($U6:$U304)*AB3)))/AB3</f>
-        <v>0.21254097982085307</v>
+        <v>0.20311582651739446</v>
       </c>
       <c r="AC5" s="3">
         <f>-(((MAX(X6:X304)-MAX($U6:$U304)*AC3)))/AC3</f>
-        <v>0.26148566728274253</v>
-      </c>
-    </row>
-    <row r="6" spans="4:29" x14ac:dyDescent="0.35">
+        <v>0.25794423633329921</v>
+      </c>
+      <c r="AG5">
+        <v>1134</v>
+      </c>
+      <c r="AH5" s="12">
+        <v>50.982999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="4:34" x14ac:dyDescent="0.35">
       <c r="D6" s="1">
         <v>43077</v>
       </c>
@@ -1723,7 +1994,7 @@
         <v>0</v>
       </c>
       <c r="Z6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="AA6">
         <f>AA5*60</f>
@@ -1731,14 +2002,21 @@
       </c>
       <c r="AB6" s="3">
         <f t="shared" ref="AB6:AC6" si="4">AB5*60</f>
-        <v>12.752458789251184</v>
+        <v>12.186949591043668</v>
       </c>
       <c r="AC6" s="3">
         <f t="shared" si="4"/>
-        <v>15.689140036964552</v>
-      </c>
-    </row>
-    <row r="7" spans="4:29" x14ac:dyDescent="0.35">
+        <v>15.476654179997952</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>21</v>
+      </c>
+      <c r="AH6">
+        <f>AG5/60+AH5/(60*60)</f>
+        <v>18.914161944444444</v>
+      </c>
+    </row>
+    <row r="7" spans="4:34" x14ac:dyDescent="0.35">
       <c r="D7" s="1">
         <v>43077</v>
       </c>
@@ -1795,8 +2073,11 @@
         <f t="shared" si="3"/>
         <v>2055.9515226541225</v>
       </c>
-    </row>
-    <row r="8" spans="4:29" x14ac:dyDescent="0.35">
+      <c r="AH7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="4:34" x14ac:dyDescent="0.35">
       <c r="D8" s="1">
         <v>43077</v>
       </c>
@@ -1854,8 +2135,11 @@
         <v>4218.2936370388707</v>
       </c>
       <c r="AB8" s="9"/>
-    </row>
-    <row r="9" spans="4:29" x14ac:dyDescent="0.35">
+      <c r="AH8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="4:34" x14ac:dyDescent="0.35">
       <c r="D9" s="1">
         <v>43077</v>
       </c>
@@ -1916,10 +2200,10 @@
         <v>4218.2936370388707</v>
       </c>
       <c r="Z9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="4:29" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="4:34" x14ac:dyDescent="0.35">
       <c r="D10" s="1">
         <v>43077</v>
       </c>
@@ -1980,13 +2264,16 @@
         <v>4218.2936370388707</v>
       </c>
       <c r="AA10" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AB10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="4:29" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="4:34" x14ac:dyDescent="0.35">
       <c r="D11" s="1">
         <v>43077</v>
       </c>
@@ -2047,7 +2334,7 @@
         <v>4218.2936370388707</v>
       </c>
       <c r="Z11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="AA11" s="8">
         <v>1000000</v>
@@ -2057,7 +2344,7 @@
       </c>
       <c r="AC11" s="10"/>
     </row>
-    <row r="12" spans="4:29" x14ac:dyDescent="0.35">
+    <row r="12" spans="4:34" x14ac:dyDescent="0.35">
       <c r="D12" s="1">
         <v>43077</v>
       </c>
@@ -2118,7 +2405,7 @@
         <v>4218.2936370388707</v>
       </c>
     </row>
-    <row r="13" spans="4:29" x14ac:dyDescent="0.35">
+    <row r="13" spans="4:34" x14ac:dyDescent="0.35">
       <c r="D13" s="1">
         <v>43077</v>
       </c>
@@ -2179,18 +2466,18 @@
         <v>4218.2936370388707</v>
       </c>
       <c r="Z13" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="AA13">
         <f>$AC5+AA11/$AC3</f>
-        <v>47.956937612570997</v>
+        <v>49.675922666522872</v>
       </c>
       <c r="AB13">
         <f>$AC5+AB11/$AC3</f>
-        <v>2786.8210947687749</v>
-      </c>
-    </row>
-    <row r="14" spans="4:29" x14ac:dyDescent="0.35">
+        <v>2887.4544596394917</v>
+      </c>
+    </row>
+    <row r="14" spans="4:34" x14ac:dyDescent="0.35">
       <c r="D14" s="1">
         <v>43077</v>
       </c>
@@ -2251,7 +2538,7 @@
         <v>4218.2936370388707</v>
       </c>
     </row>
-    <row r="15" spans="4:29" x14ac:dyDescent="0.35">
+    <row r="15" spans="4:34" x14ac:dyDescent="0.35">
       <c r="D15" s="1">
         <v>43077</v>
       </c>
@@ -2312,18 +2599,18 @@
         <v>6413.2995295865312</v>
       </c>
       <c r="Z15" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="AA15">
         <f>ROUNDDOWN(AA13/24,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB15">
         <f>ROUNDDOWN(AB13/24,0)</f>
-        <v>116</v>
-      </c>
-    </row>
-    <row r="16" spans="4:29" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="4:34" x14ac:dyDescent="0.35">
       <c r="D16" s="1">
         <v>43077</v>
       </c>
@@ -2393,15 +2680,15 @@
         <v>6413.2995295865312</v>
       </c>
       <c r="Z16" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="AA16" s="8">
         <f>ROUNDDOWN(MOD(AA13,24),0)</f>
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="AB16" s="8">
         <f>ROUNDDOWN(MOD(AB13,24),0)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="4:28" x14ac:dyDescent="0.35">
@@ -2474,15 +2761,15 @@
         <v>10494.405298341173</v>
       </c>
       <c r="Z17" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="AA17">
         <f>ROUND(MOD((MOD(AA13,24*60)),1)*60,0)</f>
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="AB17">
         <f t="shared" ref="AB17" si="11">ROUND(MOD((MOD(AB13,24*60)),1)*60,0)</f>
-        <v>49</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="4:28" x14ac:dyDescent="0.35">
@@ -2490,7 +2777,7 @@
         <v>43077</v>
       </c>
       <c r="E18" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F18">
         <v>28029</v>
@@ -2536,7 +2823,7 @@
         <v>43077</v>
       </c>
       <c r="E19" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F19">
         <v>31530</v>
@@ -2577,7 +2864,7 @@
         <v>16250.696261450854</v>
       </c>
       <c r="Z19" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="4:28" x14ac:dyDescent="0.35">
@@ -2585,7 +2872,7 @@
         <v>43077</v>
       </c>
       <c r="E20" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F20">
         <v>33163</v>
@@ -2626,7 +2913,7 @@
         <v>18359.843079970291</v>
       </c>
       <c r="Z20" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="4:28" x14ac:dyDescent="0.35">
@@ -2634,7 +2921,7 @@
         <v>43077</v>
       </c>
       <c r="E21" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F21">
         <v>41878</v>
@@ -2680,7 +2967,7 @@
         <v>43077</v>
       </c>
       <c r="E22" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F22">
         <v>43484</v>
@@ -2726,7 +3013,7 @@
         <v>43077</v>
       </c>
       <c r="E23" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F23">
         <v>45666</v>
@@ -2772,7 +3059,7 @@
         <v>43077</v>
       </c>
       <c r="E24" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F24">
         <v>46460</v>
@@ -2818,7 +3105,7 @@
         <v>43077</v>
       </c>
       <c r="E25" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F25">
         <v>49728</v>
@@ -2864,7 +3151,7 @@
         <v>43077</v>
       </c>
       <c r="E26" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F26">
         <v>55163</v>
@@ -2910,7 +3197,7 @@
         <v>43077</v>
       </c>
       <c r="E27" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F27">
         <v>60276</v>
@@ -2951,7 +3238,7 @@
         <v>31892.912998266896</v>
       </c>
       <c r="Z27" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="4:28" x14ac:dyDescent="0.35">
@@ -2959,7 +3246,7 @@
         <v>43077</v>
       </c>
       <c r="E28" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F28">
         <v>64320</v>
@@ -3005,7 +3292,7 @@
         <v>43077</v>
       </c>
       <c r="E29" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F29">
         <v>67320</v>
@@ -3045,13 +3332,22 @@
         <f t="shared" si="3"/>
         <v>34222.307006684823</v>
       </c>
+      <c r="Z29" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="30" spans="4:28" x14ac:dyDescent="0.35">
       <c r="D30" s="1">
         <v>43077</v>
       </c>
       <c r="E30" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F30">
         <v>67844</v>
@@ -3091,13 +3387,22 @@
         <f t="shared" si="3"/>
         <v>34222.307006684823</v>
       </c>
+      <c r="Z30">
+        <v>230920</v>
+      </c>
+      <c r="AA30">
+        <v>430084</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="31" spans="4:28" x14ac:dyDescent="0.35">
       <c r="D31" s="1">
         <v>43077</v>
       </c>
       <c r="E31" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F31">
         <v>69473</v>
@@ -3137,13 +3442,22 @@
         <f t="shared" si="3"/>
         <v>36559.167021539986</v>
       </c>
+      <c r="Z31">
+        <v>226888</v>
+      </c>
+      <c r="AA31">
+        <v>439920</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="32" spans="4:28" x14ac:dyDescent="0.35">
       <c r="D32" s="1">
         <v>43077</v>
       </c>
       <c r="E32" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F32">
         <v>70021</v>
@@ -3183,13 +3497,22 @@
         <f t="shared" si="3"/>
         <v>36559.167021539986</v>
       </c>
-    </row>
-    <row r="33" spans="4:28" x14ac:dyDescent="0.35">
+      <c r="Z32">
+        <v>207317</v>
+      </c>
+      <c r="AA32">
+        <v>222145</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="4:25" x14ac:dyDescent="0.35">
       <c r="D33" s="1">
         <v>43077</v>
       </c>
       <c r="E33" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F33">
         <v>96847</v>
@@ -3230,12 +3553,12 @@
         <v>48253.732854666996</v>
       </c>
     </row>
-    <row r="34" spans="4:28" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:25" x14ac:dyDescent="0.35">
       <c r="D34" s="1">
         <v>43078</v>
       </c>
       <c r="E34" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F34">
         <v>409892</v>
@@ -3300,12 +3623,12 @@
         <v>194083.50358999753</v>
       </c>
     </row>
-    <row r="35" spans="4:28" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:25" x14ac:dyDescent="0.35">
       <c r="D35" s="1">
         <v>43078</v>
       </c>
       <c r="E35" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F35">
         <v>423119</v>
@@ -3346,12 +3669,12 @@
         <v>201099.68313939095</v>
       </c>
     </row>
-    <row r="36" spans="4:28" x14ac:dyDescent="0.35">
+    <row r="36" spans="4:25" x14ac:dyDescent="0.35">
       <c r="D36" s="1">
         <v>43078</v>
       </c>
       <c r="E36" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F36">
         <v>427128</v>
@@ -3392,12 +3715,12 @@
         <v>205278.78024263433</v>
       </c>
     </row>
-    <row r="37" spans="4:28" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:25" x14ac:dyDescent="0.35">
       <c r="D37" s="1">
         <v>43078</v>
       </c>
       <c r="E37" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F37">
         <v>428751</v>
@@ -3437,22 +3760,13 @@
         <f t="shared" si="3"/>
         <v>205278.78024263433</v>
       </c>
-      <c r="Z37" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA37" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB37" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="38" spans="4:28" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="4:25" x14ac:dyDescent="0.35">
       <c r="D38" s="1">
         <v>43078</v>
       </c>
       <c r="E38" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F38">
         <v>571245</v>
@@ -3492,22 +3806,13 @@
         <f>IF(J38="","",J38*X$3/X$4)</f>
         <v>289834.10289675661</v>
       </c>
-      <c r="Z38">
-        <v>230920</v>
-      </c>
-      <c r="AA38">
-        <v>430084</v>
-      </c>
-      <c r="AB38" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="4:28" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="4:25" x14ac:dyDescent="0.35">
       <c r="D39" s="1">
         <v>43078</v>
       </c>
       <c r="E39" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F39">
         <v>576724</v>
@@ -3547,221 +3852,422 @@
         <f t="shared" ref="X39:X102" si="17">IF(J39="","",J39*X$3/X$4)</f>
         <v>292176.5624164397</v>
       </c>
-      <c r="Z39">
-        <v>226888</v>
-      </c>
-      <c r="AA39">
-        <v>439920</v>
-      </c>
-      <c r="AB39" t="s">
+    </row>
+    <row r="40" spans="4:25" x14ac:dyDescent="0.35">
+      <c r="D40" s="1">
+        <v>43078</v>
+      </c>
+      <c r="E40" t="s">
+        <v>72</v>
+      </c>
+      <c r="F40">
+        <v>673875</v>
+      </c>
+      <c r="G40" t="s">
+        <v>6</v>
+      </c>
+      <c r="H40">
+        <v>693433</v>
+      </c>
+      <c r="I40" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="40" spans="4:28" x14ac:dyDescent="0.35">
-      <c r="N40" s="2" t="str">
+      <c r="J40">
+        <v>368062</v>
+      </c>
+      <c r="K40" t="s">
+        <v>3</v>
+      </c>
+      <c r="N40" s="2">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="U40" s="5" t="str">
+        <v>23.685034722222223</v>
+      </c>
+      <c r="U40" s="5">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="V40" t="str">
+        <v>16.440762731611112</v>
+      </c>
+      <c r="V40" s="8">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="W40" t="str">
+        <v>361815.86620288127</v>
+      </c>
+      <c r="W40" s="8">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="X40" t="str">
+        <v>357636.90330969269</v>
+      </c>
+      <c r="X40" s="8">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="Z40">
-        <v>207317</v>
-      </c>
-      <c r="AA40">
-        <v>222145</v>
-      </c>
-      <c r="AB40" t="s">
+        <v>343494.15766278782</v>
+      </c>
+    </row>
+    <row r="41" spans="4:25" x14ac:dyDescent="0.35">
+      <c r="D41" s="1">
+        <v>43078</v>
+      </c>
+      <c r="E41" t="s">
+        <v>81</v>
+      </c>
+      <c r="F41">
+        <v>693768</v>
+      </c>
+      <c r="G41" t="s">
+        <v>6</v>
+      </c>
+      <c r="H41">
+        <v>713962</v>
+      </c>
+      <c r="I41" t="s">
+        <v>7</v>
+      </c>
+      <c r="J41">
+        <v>381179</v>
+      </c>
+      <c r="K41" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="4:28" x14ac:dyDescent="0.35">
-      <c r="N41" s="2" t="str">
+      <c r="N41" s="2">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="U41" s="5" t="str">
+        <v>23.744745370370371</v>
+      </c>
+      <c r="U41" s="5">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="V41" t="str">
+        <v>17.873713833666667</v>
+      </c>
+      <c r="V41">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="W41" t="str">
+        <v>372496.78332604794</v>
+      </c>
+      <c r="W41">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="X41" t="str">
+        <v>368224.70052736864</v>
+      </c>
+      <c r="X41">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-    </row>
-    <row r="42" spans="4:28" x14ac:dyDescent="0.35">
-      <c r="N42" s="2" t="str">
+        <v>355735.60846744245</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="4:25" x14ac:dyDescent="0.35">
+      <c r="D42" s="1">
+        <v>43078</v>
+      </c>
+      <c r="E42" t="s">
+        <v>82</v>
+      </c>
+      <c r="F42">
+        <v>696380</v>
+      </c>
+      <c r="G42" t="s">
+        <v>6</v>
+      </c>
+      <c r="H42">
+        <v>716772</v>
+      </c>
+      <c r="I42" t="s">
+        <v>7</v>
+      </c>
+      <c r="J42">
+        <v>383298</v>
+      </c>
+      <c r="K42" t="s">
+        <v>3</v>
+      </c>
+      <c r="N42" s="2">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="U42" s="5" t="str">
+        <v>23.748252314814813</v>
+      </c>
+      <c r="U42" s="5">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="V42" t="str">
+        <v>17.95790198572222</v>
+      </c>
+      <c r="V42">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="W42" t="str">
+        <v>373899.21410701168</v>
+      </c>
+      <c r="W42">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="X42" t="str">
+        <v>369673.95330060011</v>
+      </c>
+      <c r="X42">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-    </row>
-    <row r="43" spans="4:28" x14ac:dyDescent="0.35">
-      <c r="N43" s="2" t="str">
+        <v>357713.1669225056</v>
+      </c>
+    </row>
+    <row r="43" spans="4:25" x14ac:dyDescent="0.35">
+      <c r="D43" s="1">
+        <v>43078</v>
+      </c>
+      <c r="E43" t="s">
+        <v>85</v>
+      </c>
+      <c r="F43">
+        <v>698573</v>
+      </c>
+      <c r="G43" t="s">
+        <v>6</v>
+      </c>
+      <c r="H43">
+        <v>719092</v>
+      </c>
+      <c r="I43" t="s">
+        <v>7</v>
+      </c>
+      <c r="J43">
+        <v>383298</v>
+      </c>
+      <c r="K43" t="s">
+        <v>3</v>
+      </c>
+      <c r="N43" s="2">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="U43" s="5" t="str">
+        <v>23.751423611111111</v>
+      </c>
+      <c r="U43" s="5">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="V43" t="str">
+        <v>18.034038486222222</v>
+      </c>
+      <c r="V43">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="W43" t="str">
+        <v>375076.67609118216</v>
+      </c>
+      <c r="W43">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="X43" t="str">
+        <v>370870.48939807236</v>
+      </c>
+      <c r="X43">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-    </row>
-    <row r="44" spans="4:28" x14ac:dyDescent="0.35">
-      <c r="N44" s="2" t="str">
+        <v>357713.1669225056</v>
+      </c>
+    </row>
+    <row r="44" spans="4:25" x14ac:dyDescent="0.35">
+      <c r="D44" s="1">
+        <v>43078</v>
+      </c>
+      <c r="E44" t="s">
+        <v>86</v>
+      </c>
+      <c r="F44">
+        <v>699369</v>
+      </c>
+      <c r="G44" t="s">
+        <v>6</v>
+      </c>
+      <c r="H44">
+        <v>719721</v>
+      </c>
+      <c r="I44" t="s">
+        <v>7</v>
+      </c>
+      <c r="J44">
+        <v>383298</v>
+      </c>
+      <c r="K44" t="s">
+        <v>3</v>
+      </c>
+      <c r="N44" s="2">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="U44" s="5" t="str">
+        <v>23.752314814814817</v>
+      </c>
+      <c r="U44" s="5">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="V44" t="str">
+        <v>18.055382929055558</v>
+      </c>
+      <c r="V44">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="W44" t="str">
+        <v>375504.06311325228</v>
+      </c>
+      <c r="W44">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="X44" t="str">
+        <v>371194.89509001636</v>
+      </c>
+      <c r="X44">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-    </row>
-    <row r="45" spans="4:28" x14ac:dyDescent="0.35">
-      <c r="N45" s="2" t="str">
+        <v>357713.1669225056</v>
+      </c>
+    </row>
+    <row r="45" spans="4:25" x14ac:dyDescent="0.35">
+      <c r="D45" s="1">
+        <v>43078</v>
+      </c>
+      <c r="E45" t="s">
+        <v>87</v>
+      </c>
+      <c r="F45">
+        <v>700221</v>
+      </c>
+      <c r="G45" t="s">
+        <v>6</v>
+      </c>
+      <c r="H45">
+        <v>720709</v>
+      </c>
+      <c r="I45" t="s">
+        <v>7</v>
+      </c>
+      <c r="J45">
+        <v>385331</v>
+      </c>
+      <c r="K45" t="s">
+        <v>3</v>
+      </c>
+      <c r="N45" s="2">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="U45" s="5" t="str">
+        <v>23.753564814814816</v>
+      </c>
+      <c r="U45" s="5">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="V45" t="str">
+        <v>18.085467339499999</v>
+      </c>
+      <c r="V45">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="W45" t="str">
+        <v>375961.51756401075</v>
+      </c>
+      <c r="W45">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="X45" t="str">
+        <v>371704.45442807785</v>
+      </c>
+      <c r="X45">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-    </row>
-    <row r="46" spans="4:28" x14ac:dyDescent="0.35">
-      <c r="N46" s="2" t="str">
+        <v>359610.4658083684</v>
+      </c>
+    </row>
+    <row r="46" spans="4:25" x14ac:dyDescent="0.35">
+      <c r="D46" s="1">
+        <v>43078</v>
+      </c>
+      <c r="E46" t="s">
+        <v>88</v>
+      </c>
+      <c r="F46">
+        <v>720074</v>
+      </c>
+      <c r="G46" t="s">
+        <v>6</v>
+      </c>
+      <c r="H46">
+        <v>741278</v>
+      </c>
+      <c r="I46" t="s">
+        <v>7</v>
+      </c>
+      <c r="J46">
+        <v>398694</v>
+      </c>
+      <c r="K46" t="s">
+        <v>3</v>
+      </c>
+      <c r="N46" s="2">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="U46" s="5" t="str">
+        <v>23.7815625</v>
+      </c>
+      <c r="U46" s="5">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="V46" t="str">
+        <v>18.757350827555555</v>
+      </c>
+      <c r="V46">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="W46" t="str">
+        <v>386620.95795239997</v>
+      </c>
+      <c r="W46">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="X46" t="str">
+        <v>382312.88157846883</v>
+      </c>
+      <c r="X46">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-    </row>
-    <row r="47" spans="4:28" x14ac:dyDescent="0.35">
-      <c r="N47" s="2" t="str">
+        <v>372081.49631096807</v>
+      </c>
+    </row>
+    <row r="47" spans="4:25" x14ac:dyDescent="0.35">
+      <c r="D47" s="1">
+        <v>43078</v>
+      </c>
+      <c r="E47" t="s">
+        <v>89</v>
+      </c>
+      <c r="F47">
+        <v>746423</v>
+      </c>
+      <c r="G47" t="s">
+        <v>6</v>
+      </c>
+      <c r="H47">
+        <v>769110</v>
+      </c>
+      <c r="I47" t="s">
+        <v>7</v>
+      </c>
+      <c r="J47">
+        <v>415117</v>
+      </c>
+      <c r="K47" t="s">
+        <v>3</v>
+      </c>
+      <c r="N47" s="2">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="U47" s="5" t="str">
+        <v>23.809409722222224</v>
+      </c>
+      <c r="U47" s="5">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="V47" t="str">
+        <v>19.425692068416666</v>
+      </c>
+      <c r="V47">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="W47" t="str">
+        <v>400768.22006863775</v>
+      </c>
+      <c r="W47">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="X47" t="str">
+        <v>396667.18876159302</v>
+      </c>
+      <c r="X47">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-    </row>
-    <row r="48" spans="4:28" x14ac:dyDescent="0.35">
-      <c r="N48" s="2" t="str">
+        <v>387408.27427581087</v>
+      </c>
+    </row>
+    <row r="48" spans="4:25" x14ac:dyDescent="0.35">
+      <c r="D48" s="1">
+        <v>43078</v>
+      </c>
+      <c r="E48" t="s">
+        <v>90</v>
+      </c>
+      <c r="F48">
+        <v>767857</v>
+      </c>
+      <c r="G48" t="s">
+        <v>6</v>
+      </c>
+      <c r="H48">
+        <v>790885</v>
+      </c>
+      <c r="I48" t="s">
+        <v>7</v>
+      </c>
+      <c r="J48">
+        <v>427468</v>
+      </c>
+      <c r="K48" t="s">
+        <v>3</v>
+      </c>
+      <c r="N48" s="2">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="U48" s="5" t="str">
+        <v>23.8321875</v>
+      </c>
+      <c r="U48" s="5">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="V48" t="str">
+        <v>19.972498293999998</v>
+      </c>
+      <c r="V48">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="W48" t="str">
+        <v>412276.52839910344</v>
+      </c>
+      <c r="W48">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="X48" t="str">
+        <v>407897.60838334245</v>
+      </c>
+      <c r="X48">
         <f t="shared" si="17"/>
-        <v/>
+        <v>398934.8549641</v>
       </c>
     </row>
     <row r="49" spans="14:24" x14ac:dyDescent="0.35">

</xml_diff>